<commit_message>
doc: Actualización de README.md
</commit_message>
<xml_diff>
--- a/scripts/00_forums_basicsciences/Ciencias_Basicas.xlsx
+++ b/scripts/00_forums_basicsciences/Ciencias_Basicas.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://poligran-my.sharepoint.com/personal/ceguzman_poligran_edu_co/Documents/My Workspace/1 - Productividad/1 - Automatizaciones/apicanvas/3 - API Canvas LMS/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://poligran-my.sharepoint.com/personal/cedguzman_poligran_edu_co/Documents/1 - Engineer Sytems/Programmer/2 - Python/00_scripts_apicanvas/scripts/00_forums_basicsciences/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="34" documentId="13_ncr:1_{DF85428B-50A2-4E4E-9E0F-2AF1A00121DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9CCF205C-CC33-40CD-964B-C8680B9AB55F}"/>
+  <xr:revisionPtr revIDLastSave="38" documentId="13_ncr:1_{DF85428B-50A2-4E4E-9E0F-2AF1A00121DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8E242D04-5D39-47E3-9A43-09FF6D71AF13}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{5DC6F971-87C6-4698-BEE8-154CC66E0840}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{5DC6F971-87C6-4698-BEE8-154CC66E0840}"/>
   </bookViews>
   <sheets>
     <sheet name="Foros" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="136">
   <si>
     <t>canvas_section_id</t>
   </si>
@@ -444,6 +444,9 @@
   </si>
   <si>
     <t>SEGUNDO BLOQUE-TEORICO - VIRTUAL/RAZONAMIENTO VARIACIONAL-[GRUPO C01]</t>
+  </si>
+  <si>
+    <t>87524</t>
   </si>
 </sst>
 </file>
@@ -838,7 +841,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1156,30 +1159,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{180A677A-70DB-4E07-80FF-C7DEDFC168D4}">
   <dimension ref="A1:P27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:P27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.140625" customWidth="1"/>
-    <col min="2" max="2" width="18.5703125" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" customWidth="1"/>
-    <col min="5" max="5" width="25.140625" customWidth="1"/>
-    <col min="6" max="6" width="16.7109375" customWidth="1"/>
-    <col min="7" max="7" width="18.28515625" customWidth="1"/>
-    <col min="8" max="8" width="42.7109375" customWidth="1"/>
-    <col min="9" max="9" width="29.7109375" customWidth="1"/>
-    <col min="10" max="10" width="39.5703125" customWidth="1"/>
-    <col min="11" max="11" width="63.7109375" customWidth="1"/>
-    <col min="12" max="12" width="31.140625" customWidth="1"/>
-    <col min="13" max="13" width="32.85546875" customWidth="1"/>
-    <col min="14" max="14" width="27.7109375" customWidth="1"/>
-    <col min="15" max="15" width="47.42578125" customWidth="1"/>
+    <col min="1" max="1" width="19.109375" customWidth="1"/>
+    <col min="2" max="2" width="18.5546875" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" customWidth="1"/>
+    <col min="5" max="5" width="25.109375" customWidth="1"/>
+    <col min="6" max="6" width="16.6640625" customWidth="1"/>
+    <col min="7" max="7" width="18.33203125" customWidth="1"/>
+    <col min="8" max="8" width="42.6640625" customWidth="1"/>
+    <col min="9" max="9" width="29.6640625" customWidth="1"/>
+    <col min="10" max="10" width="39.5546875" customWidth="1"/>
+    <col min="11" max="11" width="63.6640625" customWidth="1"/>
+    <col min="12" max="12" width="31.109375" customWidth="1"/>
+    <col min="13" max="13" width="32.88671875" customWidth="1"/>
+    <col min="14" max="14" width="27.6640625" customWidth="1"/>
+    <col min="15" max="15" width="47.44140625" customWidth="1"/>
     <col min="16" max="16" width="49" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1229,7 +1232,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>100</v>
       </c>
@@ -1279,7 +1282,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>105</v>
       </c>
@@ -1329,7 +1332,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>109</v>
       </c>
@@ -1379,7 +1382,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>113</v>
       </c>
@@ -1429,7 +1432,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>28</v>
       </c>
@@ -1479,7 +1482,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>33</v>
       </c>
@@ -1529,7 +1532,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>37</v>
       </c>
@@ -1579,7 +1582,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>41</v>
       </c>
@@ -1629,7 +1632,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>45</v>
       </c>
@@ -1679,7 +1682,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>49</v>
       </c>
@@ -1729,7 +1732,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>53</v>
       </c>
@@ -1779,7 +1782,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>58</v>
       </c>
@@ -1829,9 +1832,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>87524</v>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>135</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>22</v>
@@ -1879,7 +1882,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>62</v>
       </c>
@@ -1929,7 +1932,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>66</v>
       </c>
@@ -1979,7 +1982,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>71</v>
       </c>
@@ -2029,7 +2032,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>74</v>
       </c>
@@ -2079,7 +2082,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>81</v>
       </c>
@@ -2129,7 +2132,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>85</v>
       </c>
@@ -2179,7 +2182,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>88</v>
       </c>
@@ -2229,7 +2232,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>92</v>
       </c>
@@ -2279,7 +2282,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>96</v>
       </c>
@@ -2329,7 +2332,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>118</v>
       </c>
@@ -2379,7 +2382,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>123</v>
       </c>
@@ -2429,7 +2432,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>127</v>
       </c>
@@ -2479,7 +2482,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>131</v>
       </c>

</xml_diff>